<commit_message>
updates from last time I taught Adv Spring
</commit_message>
<xml_diff>
--- a/0Docs/AdvancedSpring_Overview.xlsx
+++ b/0Docs/AdvancedSpring_Overview.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbirze\Documents\ContractInstructor\ClassMaterials\Spring\SpringAdvanced\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbirze\Documents\ContractInstructor\ClassMaterials\Spring\workspaceSpring\AdvSpring\0Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Day 3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="99">
   <si>
     <t>Topic</t>
   </si>
@@ -336,14 +335,6 @@
 Tools: Spring XD Command Shell, DSL, and Web GUI</t>
   </si>
   <si>
-    <t>Spring XD Modules Overview
-Sources: HTTP, JDBC, JMS
-Sinks: JDBC, HDFS, File
-Processors: Filter, Transform
-Taps, Counters, and Gauges
-Rich Guage Analitic and XD Jobs</t>
-  </si>
-  <si>
     <t xml:space="preserve">19 slides, </t>
   </si>
   <si>
@@ -391,56 +382,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">What is the Spring Framework?
-Spring Architecture
- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  Extra Slide: The Application Context</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Spring Hello, World
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> DEMO: SpringDemos/SpringJavaDemos, 
-                            pkg XMLAnnotations.hello 
-</t>
-    </r>
-  </si>
-  <si>
     <t>40 min</t>
   </si>
   <si>
     <t>120  min</t>
-  </si>
-  <si>
-    <t>45-60 min</t>
   </si>
   <si>
     <t>Lab 8 Debrief, Demo</t>
@@ -479,23 +424,6 @@
       </rPr>
       <t xml:space="preserve"> - Part 1:  Project and Database Setup (20 min)
  - Part 2: Building the Application       (70 min)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Lab 6: Messages and Channels
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Part 1:  Using Point-t-Point Channels                  (30 min)
- - Part 2: Adding a Publish-Subscribe Channel   (20 min)</t>
     </r>
   </si>
   <si>
@@ -592,59 +520,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Hadoop Overview
- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> SHOW WEBSITE: Wikipedia release History table</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Components: HDFS, YARN
-MapReduce
-Phases: Map and Reduce
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  SHOW WEBSITE: MapReduce Alternatives</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Installation and Conffiguration</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Remote Objects
 RMI and Spring 
 </t>
@@ -775,8 +650,9 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Different Endpoints: Messaging, Inbound, Outbound
-  </t>
+      <t xml:space="preserve">What is the Spring Framework?
+Spring Architecture
+ </t>
     </r>
     <r>
       <rPr>
@@ -787,7 +663,141 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">  DEMO: lab07\src\test\java\com\demo\SJDBCOutbound</t>
+      <t xml:space="preserve">  Extra Slide: The Application Context</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Spring Hello, World
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DEMO: AdvSpring/AA_SpringJavaDemos, 
+                            pkg XMLAnnotations.hello 
+</t>
+    </r>
+  </si>
+  <si>
+    <t>if need to kill embedded tomcat to free port 8080</t>
+  </si>
+  <si>
+    <t>C:%&gt; netstat -ano</t>
+  </si>
+  <si>
+    <t>look at top of processes to find the one holding port 8080</t>
+  </si>
+  <si>
+    <t>C:%&gt; taskkill /F /PID xxxx</t>
+  </si>
+  <si>
+    <t>where xxxx is the pid of the taks holding 8080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90 min total 30 min today
+60 min tomorrow </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lab 6: Messages and Channels
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Part 1:  Using Point-to-Point Channels                (60 min)
+ - Part 2: Adding a Publish-Subscribe Channel   (30 min)</t>
+    </r>
+  </si>
+  <si>
+    <t>90 min total 
+60 min today
+ 30 min yesterday</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Download Your Labs!!!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Review
+What did you learn?
+Q&amp;A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hadoop Overview
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SHOW WEBSITE: Wikipedia release History table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Components: HDFS, YARN
+MapReduce
+Phases: Map and Reduce
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SHOW wrkspc: AdvSpring/0Docs/Lab07MsgFlow.jpg</t>
     </r>
     <r>
       <rPr>
@@ -802,13 +812,72 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Gateways and Routers
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  SHOW WEBSITE: MapReduce Alternatives</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Installation and Conffiguration</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   SHOW wrkspc: AdvSpring/0Docs/Lab07MsgFlow.jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Different Endpoints: Messaging, Inbound, Outbound
+  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  DEMO: lab07\src\test\java\com\demo\SJDBCOutbound</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Gateways and Routers
 </t>
     </r>
     <r>
@@ -833,13 +902,76 @@
       <t xml:space="preserve">
 Splitters, Aggregators, Filters, and Transformers</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Spring XD Modules Overview
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Spring XD cmd prompt: %&gt; module list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Sources: HTTP, JDBC, JMS
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  SHOW WEBSITE: Spring XD doc: Sources, Process, and 
+                               Sinks sections</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Sinks: JDBC, HDFS, File
+Processors: Filter, Transform
+Taps, Counters, and Gauges
+Rich Guage Analitic and XD Jobs</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Stuff they want to see:  </t>
+  </si>
+  <si>
+    <t>Spring Cloud Flow
+Integration with AWS
+Hadoop working example</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -907,6 +1039,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1081,7 +1227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1209,6 +1355,11 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1493,10 +1644,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1559,7 +1710,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="24" t="s">
@@ -1569,7 +1720,7 @@
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="31"/>
       <c r="B5" s="35" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="15" t="s">
@@ -1600,7 +1751,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="24" t="s">
@@ -1610,7 +1761,7 @@
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="31"/>
       <c r="B8" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="15" t="s">
@@ -1628,7 +1779,7 @@
         <v>40</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1667,13 +1818,13 @@
         <v>39</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="31"/>
       <c r="B13" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="15" t="s">
@@ -1693,7 +1844,7 @@
       <c r="E14" s="22"/>
     </row>
     <row r="15" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="40" t="s">
         <v>5</v>
       </c>
@@ -1703,9 +1854,30 @@
       <c r="D15" s="12"/>
       <c r="E15" s="24"/>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="62" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="62" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1714,10 +1886,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D18" sqref="C18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1780,7 +1952,7 @@
         <v>51</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="24" t="s">
@@ -1790,7 +1962,7 @@
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="31"/>
       <c r="B5" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="15" t="s">
@@ -1830,7 +2002,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="24" t="s">
@@ -1840,7 +2012,7 @@
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="31"/>
       <c r="B9" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15" t="s">
@@ -1852,10 +2024,10 @@
       <c r="A10" s="42"/>
       <c r="B10" s="43"/>
       <c r="C10" s="20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>37</v>
@@ -1880,7 +2052,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="24" t="s">
@@ -1906,19 +2078,19 @@
       <c r="A14" s="30"/>
       <c r="B14" s="39"/>
       <c r="C14" s="20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="15" t="s">
@@ -1952,55 +2124,44 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30"/>
       <c r="B18" s="43"/>
       <c r="C18" s="20" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="22"/>
-    </row>
-    <row r="20" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
-      <c r="B20" s="40" t="s">
+    <row r="19" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27"/>
+      <c r="B19" s="40" t="s">
         <v>5</v>
       </c>
+      <c r="C19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="24"/>
+    </row>
+    <row r="20" spans="1:5" ht="55.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18"/>
+      <c r="B20" s="17" t="s">
+        <v>3</v>
+      </c>
       <c r="C20" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D20" s="12"/>
-      <c r="E20" s="24"/>
-    </row>
-    <row r="21" spans="1:5" ht="55.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
+      <c r="E20" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="53" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="52" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2009,10 +2170,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2067,195 +2228,227 @@
       <c r="D3" s="12"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28">
-        <v>10</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30"/>
+    <row r="4" spans="1:5" ht="118.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="32"/>
       <c r="B5" s="39"/>
       <c r="C5" s="20" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
-      <c r="B6" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
+        <v>38</v>
+      </c>
+      <c r="E5" s="22"/>
+    </row>
+    <row r="6" spans="1:5" ht="118.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28">
+        <v>10</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30"/>
       <c r="B7" s="39"/>
       <c r="C7" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="31"/>
+      <c r="B8" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D9" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="8" spans="1:5" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29">
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="1:5" ht="154.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29">
         <v>11</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B10" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="24" t="s">
+      <c r="C10" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29">
+    <row r="11" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29">
         <v>12</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B11" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C11" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="24" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15" t="s">
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="31"/>
+      <c r="B12" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11" spans="1:5" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="22" t="s">
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="30"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="32"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="22"/>
+    </row>
+    <row r="15" spans="1:5" ht="174" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29">
+        <v>13</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A16" s="31"/>
+      <c r="B16" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="32"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="20" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="21" t="s">
+      <c r="D18" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="22"/>
-    </row>
-    <row r="13" spans="1:5" ht="123" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29">
-        <v>13</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="22"/>
-    </row>
-    <row r="17" spans="1:5" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33"/>
-      <c r="B17" s="40" t="s">
+      <c r="E18" s="22"/>
+    </row>
+    <row r="19" spans="1:5" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="33"/>
+      <c r="B19" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="24"/>
-    </row>
-    <row r="18" spans="1:5" ht="55.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="17" t="s">
+      <c r="C19" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="24"/>
+    </row>
+    <row r="20" spans="1:5" ht="55.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18"/>
+      <c r="B20" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="55" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="54" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lots of updates and good extra info additions
</commit_message>
<xml_diff>
--- a/0Docs/AdvancedSpring_Overview.xlsx
+++ b/0Docs/AdvancedSpring_Overview.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12672" windowHeight="6264"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12672" windowHeight="6264" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="98">
   <si>
     <t>Topic</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>10 min</t>
-  </si>
-  <si>
-    <t>90 - 120  min</t>
   </si>
   <si>
     <t>45 min</t>
@@ -265,9 +262,6 @@
   </si>
   <si>
     <t>Lab 2 Debrief, Questions</t>
-  </si>
-  <si>
-    <t>Introduction to Spring Inegration</t>
   </si>
   <si>
     <r>
@@ -520,136 +514,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Remote Objects
-RMI and Spring 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">    DEMO: SpringDemos/RMIRemotingDemo, RMI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-HttpInvoker and Spring
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">    DEMO: SpringDemos/RMIRemotingDemo, HttpInvoker </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Messaging Service and JMS
-JmsTemplate
-    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DEMO: SpringDemos/RMIRemotingDemo, JMS Send Receive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Sending and Receiving Messages
-    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DEMO: SpringDemos/RMIRemotingDemo, MsgListener</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Batch Application Concepts
-Spring Batch Concepts
-Writing and Configuring a
-Spring Batch Application
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">    DEMO: lab04, \src\test\java\demo\springbatch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">What is the Spring Framework?
 Spring Architecture
  </t>
@@ -707,10 +571,6 @@
     <t>where xxxx is the pid of the taks holding 8080</t>
   </si>
   <si>
-    <t xml:space="preserve">90 min total 30 min today
-60 min tomorrow </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Lab 6: Messages and Channels
 </t>
@@ -726,11 +586,6 @@
       <t xml:space="preserve"> - Part 1:  Using Point-to-Point Channels                (60 min)
  - Part 2: Adding a Publish-Subscribe Channel   (30 min)</t>
     </r>
-  </si>
-  <si>
-    <t>90 min total 
-60 min today
- 30 min yesterday</t>
   </si>
   <si>
     <r>
@@ -835,76 +690,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   SHOW wrkspc: AdvSpring/0Docs/Lab07MsgFlow.jpg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Different Endpoints: Messaging, Inbound, Outbound
-  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  DEMO: lab07\src\test\java\com\demo\SJDBCOutbound</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Gateways and Routers
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   DEMO: lab07\src\test\java\com\demo\SOAPGateway</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Splitters, Aggregators, Filters, and Transformers</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Spring XD Modules Overview
    </t>
     </r>
@@ -965,6 +750,286 @@
     <t>Spring Cloud Flow
 Integration with AWS
 Hadoop working example</t>
+  </si>
+  <si>
+    <t>Introduction to Spring Integration</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Remote Objects
+RMI and Spring 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    DEMO: SpringDemos/RMIRemotingDemo, RMI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+HttpInvoker and Spring
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    DEMO: SpringDemos/RMIRemotingDemo, HttpInvoker </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Messaging Service and JMS
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SHOW: Messaging Provider Diagram on Web</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+JmsTemplate
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEMO: SpringDemos/RMIRemotingDemo, JMS Send Receive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Sending and Receiving Messages
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEMO: SpringDemos/RMIRemotingDemo, MsgListener</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>~3PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90 min </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Adapters
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    SHOW JavaDoc MessageAdapter to see all subclasses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Different Endpoints: Messaging, Inbound, Outbound
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  DEMO: lab07\src\test\java\com\demo\SJDBCOutbound</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Gateways and Routers
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   DEMO: lab07\src\test\java\com\demo\SOAPGateway</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Splitters, Aggregators, Filters, and Transformers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Batch Application Concepts
+Spring Batch Concepts
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Show: Extra slidesScaling Batch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+XML Configuration 
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SHOW: test/demo.springBatch.DemoSpringBatch.xml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Writing and Configuring a
+Spring Batch Application
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    DEMO: lab04, \src\test\java\demo\springbatch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1086,7 +1151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1223,11 +1288,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1360,6 +1434,21 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1646,8 +1735,8 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1663,7 +1752,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="25" t="s">
@@ -1710,7 +1799,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="24" t="s">
@@ -1720,7 +1809,7 @@
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="31"/>
       <c r="B5" s="35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="15" t="s">
@@ -1733,14 +1822,14 @@
         <v>3</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1751,7 +1840,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="24" t="s">
@@ -1761,7 +1850,7 @@
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="31"/>
       <c r="B8" s="35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="15" t="s">
@@ -1773,13 +1862,13 @@
       <c r="A9" s="34"/>
       <c r="B9" s="41"/>
       <c r="C9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1801,7 +1890,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="24" t="s">
@@ -1812,19 +1901,19 @@
       <c r="A12" s="42"/>
       <c r="B12" s="39"/>
       <c r="C12" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="D12" s="47">
+        <v>5.2083333333333336E-2</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="31"/>
       <c r="B13" s="35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="15" t="s">
@@ -1836,7 +1925,7 @@
       <c r="A14" s="27"/>
       <c r="B14" s="39"/>
       <c r="C14" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>38</v>
@@ -1856,23 +1945,23 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="45" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" s="44" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" s="44" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1886,16 +1975,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D18" sqref="C18:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="41.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="79.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="21.44140625" style="3" customWidth="1"/>
@@ -1905,7 +1994,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="25" t="s">
@@ -1944,25 +2033,25 @@
       <c r="D3" s="12"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="207.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="225.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29">
         <v>6</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A5" s="31"/>
       <c r="B5" s="35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="15" t="s">
@@ -1974,7 +2063,7 @@
       <c r="A6" s="30"/>
       <c r="B6" s="39"/>
       <c r="C6" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>9</v>
@@ -1994,7 +2083,7 @@
       </c>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:5" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27">
         <v>7</v>
       </c>
@@ -2002,7 +2091,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="24" t="s">
@@ -2012,7 +2101,7 @@
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="31"/>
       <c r="B9" s="35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15" t="s">
@@ -2024,79 +2113,81 @@
       <c r="A10" s="42"/>
       <c r="B10" s="43"/>
       <c r="C10" s="20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="20" t="s">
+    <row r="11" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="31"/>
+      <c r="B11" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
+      <c r="B12" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D12" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="1:5" ht="183.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="29">
+      <c r="E12" s="22"/>
+    </row>
+    <row r="13" spans="1:5" ht="170.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29">
         <v>8</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B13" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29">
-        <v>9</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>47</v>
-      </c>
       <c r="C13" s="11" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="16"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29">
+        <v>9</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="30"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32"/>
@@ -2109,55 +2200,27 @@
       </c>
       <c r="E16" s="22"/>
     </row>
-    <row r="17" spans="1:5" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="29">
-        <v>10</v>
-      </c>
-      <c r="B17" s="37" t="s">
-        <v>16</v>
+    <row r="17" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28"/>
+      <c r="B17" s="40" t="s">
+        <v>5</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="D17" s="12"/>
-      <c r="E17" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
-      <c r="B19" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="24"/>
-    </row>
-    <row r="20" spans="1:5" ht="55.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="17" t="s">
+      <c r="E17" s="24"/>
+    </row>
+    <row r="18" spans="1:5" ht="55.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2170,10 +2233,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2189,7 +2252,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="25" t="s">
@@ -2228,227 +2291,242 @@
       <c r="D3" s="12"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" ht="118.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="22" t="s">
+    <row r="4" spans="1:5" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29">
+        <v>10</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="30"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="22"/>
-    </row>
-    <row r="6" spans="1:5" ht="118.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28">
-        <v>10</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="31"/>
+      <c r="B6" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30"/>
       <c r="B7" s="39"/>
       <c r="C7" s="20" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
-      <c r="B8" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="39"/>
+        <v>38</v>
+      </c>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:5" ht="140.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="29">
+        <v>11</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="31"/>
+      <c r="B10" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="32"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="22"/>
-    </row>
-    <row r="10" spans="1:5" ht="154.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29">
-        <v>11</v>
-      </c>
-      <c r="B10" s="37" t="s">
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="1:5" ht="154.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="30">
+        <v>12</v>
+      </c>
+      <c r="B12" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="24" t="s">
+      <c r="C12" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="29">
-        <v>12</v>
-      </c>
-      <c r="B11" s="37" t="s">
+    <row r="13" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29">
+        <v>13</v>
+      </c>
+      <c r="B13" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
-      <c r="B12" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="1:5" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
+      <c r="C13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="30"/>
       <c r="B14" s="39"/>
       <c r="C14" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D14" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A15" s="31"/>
+      <c r="B15" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="32"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="22"/>
-    </row>
-    <row r="15" spans="1:5" ht="174" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="29">
-        <v>13</v>
-      </c>
-      <c r="B15" s="37" t="s">
+      <c r="E16" s="22"/>
+    </row>
+    <row r="17" spans="1:5" ht="174" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="29">
+        <v>14</v>
+      </c>
+      <c r="B17" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
-      <c r="B16" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
+      <c r="C17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30"/>
       <c r="B18" s="39"/>
       <c r="C18" s="20" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D18" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="32"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="22"/>
-    </row>
-    <row r="19" spans="1:5" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33"/>
-      <c r="B19" s="40" t="s">
+      <c r="E19" s="22"/>
+    </row>
+    <row r="20" spans="1:5" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="33"/>
+      <c r="B20" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="24"/>
-    </row>
-    <row r="20" spans="1:5" ht="55.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="17" t="s">
+      <c r="C20" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="24"/>
+    </row>
+    <row r="21" spans="1:5" ht="55.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18"/>
+      <c r="B21" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C21" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>98</v>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="54" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup scale="51" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>